<commit_message>
Ajout des regles et du menu
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -1,25 +1,198 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F924EA8-15C0-4FB4-9B93-03A3E7880134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heure début</t>
+  </si>
+  <si>
+    <t>Heure fin</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tâche</t>
+  </si>
+  <si>
+    <t>Lieu</t>
+  </si>
+  <si>
+    <t>Descriptif</t>
+  </si>
+  <si>
+    <t>Terminer</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>I-431</t>
+  </si>
+  <si>
+    <t>Théorie</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t>CPNV</t>
+  </si>
+  <si>
+    <t>M.Viret bous a montrer comment utiliser Github</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>LVT</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>J'ai installer Github et upload mes fichiers dessus</t>
+  </si>
+  <si>
+    <t>On a appris a push des dossier sur Github</t>
+  </si>
+  <si>
+    <t>J'ai push mes doccument théorique sur Github et inviter M.Viret</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>On a revu les MCD, on a repasser en vue comment stocker des données</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>Scénario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencer mes MCD, on a réfléchit comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai corriger des fautes </t>
+  </si>
+  <si>
+    <t>j'ai corriger des faute de mes scénario, il ne demmarait pas tous au meme endroits</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>Ma-20</t>
+  </si>
+  <si>
+    <t>Abscence</t>
+  </si>
+  <si>
+    <t>Maison</t>
+  </si>
+  <si>
+    <t>Abcsent</t>
+  </si>
+  <si>
+    <t>Mal de ventre</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Regle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencer mon menu, il a pour l'instant 3 choix </t>
+  </si>
+  <si>
+    <t>J'ai commencer mes regle, je me suis dit qu'il serait interessant de les mettre dans un fichier a part car elles seront suremment asser longue</t>
+  </si>
+  <si>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>Théorire</t>
+  </si>
+  <si>
+    <t>Exercice</t>
+  </si>
+  <si>
+    <t>On a vu ce qu'était une manquette</t>
+  </si>
+  <si>
+    <t>En équipe, on a du réaliser des HUD de jeux viéo</t>
+  </si>
+  <si>
+    <t>Nous avons a les un apres les autre fait corriger notre HUD par toutes la classe</t>
+  </si>
+  <si>
+    <t>Apres correction des HUD nous les avons refaire en mieux</t>
+  </si>
+  <si>
+    <t>Nous avons corriger les version 2.0 de tout les HUD de la classe</t>
+  </si>
+  <si>
+    <t>J'ai presque terminer mes regle il me reste pluqu'a mettre de la couleur</t>
+  </si>
+  <si>
+    <t>Je suis aller regarder comment fonctionais plussieur formule</t>
+  </si>
+  <si>
+    <t>https://www.learn-c.org/</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,13 +222,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +257,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L37" totalsRowShown="0">
+  <autoFilter ref="B4:L37" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A0D6E0C5-3E1B-4BB4-9947-2541E1F6859A}" name="Heure fin" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{F1972E60-CD5A-4CD7-B348-8F8E50C358F5}" name="Durée" dataDxfId="1">
+      <calculatedColumnFormula>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{60EE89D6-B68E-4AE0-806C-9F288D767390}" name="Module"/>
+    <tableColumn id="5" xr3:uid="{0F726875-2016-47DE-8658-01D6C1348E07}" name="Type"/>
+    <tableColumn id="6" xr3:uid="{C042BDDE-C9BC-46B7-A987-B94D920F832D}" name="Tâche"/>
+    <tableColumn id="7" xr3:uid="{ADC89799-1040-47E9-B2E4-CC75A0B3D9B7}" name="Lieu"/>
+    <tableColumn id="8" xr3:uid="{736704FD-0C09-4D18-9CFD-4EBB341D9FE9}" name="Descriptif" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{5AB23A3F-148F-409E-9C15-0A65AB55315F}" name="Terminer"/>
+    <tableColumn id="10" xr3:uid="{FDC8B8E5-675D-4789-BCF4-9DD634D4B7A5}" name="Source"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +543,759 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="17.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="31" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="30.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>44244</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E5" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>44244</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E6" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>44244</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E7" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>44244</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E9" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E10" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E11" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>0.11458333333333331</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E12" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>44246</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E13" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>44258</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E14" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>44258</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E15" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E16" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E17" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E18" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E19" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>40972</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E20" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>44260</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E21" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>44260</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E22" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E24" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E26" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E27" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E28" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E29" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E30" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E31" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="E32" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout des question pour la position et de la vérification
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F924EA8-15C0-4FB4-9B93-03A3E7880134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9A68DB-54B4-49D3-87DA-FE570A82AA56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>https://www.learn-c.org/</t>
+  </si>
+  <si>
+    <t>Jeu</t>
+  </si>
+  <si>
+    <t>j'ai crée 2 focntion pour demande ou le joueur voulais tirer et une troisieme qui regarde si il y a un bateau</t>
   </si>
 </sst>
 </file>
@@ -547,7 +553,7 @@
   <dimension ref="B4:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>44244</v>
       </c>
@@ -737,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>44245</v>
       </c>
@@ -1202,10 +1208,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E23" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="23" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>44261</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E23" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
J'ai terminé ma grille et je l'ai affiché dans mon jeu
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9A68DB-54B4-49D3-87DA-FE570A82AA56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED349E0-E4D0-4167-BDB6-D48D9CE9DD39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>j'ai crée 2 focntion pour demande ou le joueur voulais tirer et une troisieme qui regarde si il y a un bateau</t>
+  </si>
+  <si>
+    <t>Grille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai tester quellque manier de faire une grille et j'ai décider comment j'aillais la faire </t>
+  </si>
+  <si>
+    <t>j'ai finit ma grille et je l'ai afficher dans mon jeux</t>
   </si>
 </sst>
 </file>
@@ -552,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="87" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,16 +1250,70 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E24" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E25" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="24" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>44264</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E24" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E25" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Amélioration du code et affichage de où on a tirer sur la grille
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED349E0-E4D0-4167-BDB6-D48D9CE9DD39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5CC61F-0414-4455-8389-5606010B9346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>j'ai finit ma grille et je l'ai afficher dans mon jeux</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>J'ai améliorer les fonctions qui demande les postion ou l'on veut tirer, j'ai aussi mis en page le code</t>
+  </si>
+  <si>
+    <t>J'ai fait que lorsque qu'on tire sur une case la grille l affiche</t>
+  </si>
+  <si>
+    <t>oui</t>
   </si>
 </sst>
 </file>
@@ -561,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,7 +1259,7 @@
         <v>51</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -1316,16 +1328,70 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E26" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E27" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="26" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E26" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="E27" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Les casse touchée avec un bateau sont différente des autre
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5CC61F-0414-4455-8389-5606010B9346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A88A4-E979-4FD5-B7FB-D610F918AF1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>oui</t>
+  </si>
+  <si>
+    <t>J'ai fait que les casse tocuher avec un bateau soit différente qu'une case touchée avec rien</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="B4:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,10 +1397,37 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E28" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="28" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E28" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ajout de case de couleur
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A88A4-E979-4FD5-B7FB-D610F918AF1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4CFE39-6B9E-4980-9D4C-D169BF914F6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -214,6 +214,56 @@
   </si>
   <si>
     <t>J'ai fait que les casse tocuher avec un bateau soit différente qu'une case touchée avec rien</t>
+  </si>
+  <si>
+    <t>Cahier des charges</t>
+  </si>
+  <si>
+    <t>On a eu de la théorie sur comment remplir un chier des charges</t>
+  </si>
+  <si>
+    <t>Cas d'utilisation</t>
+  </si>
+  <si>
+    <t>On a crée nos cas d'utilisation pour la bataille navale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a eu de la théorie sur comment faire nos scénario </t>
+  </si>
+  <si>
+    <t>On a commencer a faire nos scénario</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Planification</t>
+  </si>
+  <si>
+    <t>On a parler de la planification de la bataille navale</t>
+  </si>
+  <si>
+    <t>En groupe de 2, on a décris un logo et l autre devait le dessiner sans commentaire entre 2. 
+On a refait l ex mais cette fois si en décrivant pendant que l autre dessine 
+C'était pour nous introduire Les planification Cascafe et Agile</t>
+  </si>
+  <si>
+    <t>Le prof nous a montrer comment faire des Issues et des Sprints sur github</t>
+  </si>
+  <si>
+    <t>J'ai crée mes Issues et mes Sprints</t>
+  </si>
+  <si>
+    <t>Journal de travaille</t>
+  </si>
+  <si>
+    <t>J'ai corriger mes erreur que j avais dedans</t>
+  </si>
+  <si>
+    <t>J'ai ajouter des case de couleur quand un bateau est toucher et quand une case est toucher avec rien dessus</t>
+  </si>
+  <si>
+    <t>J'ai rajouter dans mes regle les casse de couleur</t>
   </si>
 </sst>
 </file>
@@ -290,8 +340,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L37" totalsRowShown="0">
-  <autoFilter ref="B4:L37" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L41" totalsRowShown="0">
+  <autoFilter ref="B4:L41" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -574,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L37"/>
+  <dimension ref="B4:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,17 +681,17 @@
     </row>
     <row r="5" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
-        <v>44244</v>
+        <v>44238</v>
       </c>
       <c r="C5" s="3">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D5" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="E5" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>1.041666666666663E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -650,34 +700,28 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>44244</v>
+        <v>44238</v>
       </c>
       <c r="C6" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="D6" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E6" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>1.0416666666666741E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -686,31 +730,28 @@
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
-        <v>44244</v>
+        <v>44238</v>
       </c>
       <c r="C7" s="3">
-        <v>0.60416666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D7" s="3">
-        <v>0.61458333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E7" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>1.0416666666666741E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -719,30 +760,24 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <v>44244</v>
+        <v>44238</v>
       </c>
       <c r="C8" s="3">
-        <v>0.61458333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D8" s="3">
-        <v>0.625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="E8" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
@@ -755,31 +790,28 @@
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="C9" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="D9" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E9" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -788,13 +820,13 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
@@ -803,19 +835,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="C10" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="D10" s="3">
-        <v>0.375</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E10" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.0833333333333315E-2</v>
+        <v>1.0416666666666741E-2</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -824,64 +856,67 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="C11" s="3">
-        <v>0.375</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D11" s="3">
-        <v>0.48958333333333331</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="E11" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>0.11458333333333331</v>
+        <v>1.0416666666666741E-2</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>44245</v>
+        <v>44244</v>
       </c>
       <c r="C12" s="3">
-        <v>0.48958333333333331</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="D12" s="3">
-        <v>0.51041666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="E12" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.0833333333333315E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -890,109 +925,115 @@
         <v>17</v>
       </c>
       <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E13" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>44245</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E14" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
         <v>24</v>
       </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>44246</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="E13" s="3">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>44258</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="E14" s="3">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
-        <v>44258</v>
+        <v>44245</v>
       </c>
       <c r="C15" s="3">
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="D15" s="3">
-        <v>0.625</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="E15" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>6.25E-2</v>
+        <v>0.11458333333333331</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="K15" t="s">
         <v>28</v>
@@ -1000,164 +1041,161 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
-        <v>40972</v>
+        <v>44245</v>
       </c>
       <c r="C16" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="D16" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E16" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>44246</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E17" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>44258</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E18" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="1">
-        <v>40972</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="E17" s="3">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
-        <v>40972</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.44791666666666669</v>
-      </c>
-      <c r="E18" s="3">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>5.208333333333337E-2</v>
-      </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I18" t="s">
         <v>13</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
-        <v>40972</v>
+        <v>44258</v>
       </c>
       <c r="C19" s="3">
-        <v>0.44791666666666669</v>
+        <v>0.5625</v>
       </c>
       <c r="D19" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.625</v>
       </c>
       <c r="E19" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>3.125E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>40972</v>
       </c>
       <c r="C20" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D20" s="3">
-        <v>0.51041666666666663</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="E20" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>3.1249999999999944E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
         <v>39</v>
       </c>
-      <c r="H20" t="s">
-        <v>40</v>
-      </c>
       <c r="I20" t="s">
         <v>13</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K20" t="s">
         <v>15</v>
@@ -1165,152 +1203,149 @@
     </row>
     <row r="21" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>44260</v>
+        <v>40972</v>
       </c>
       <c r="C21" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D21" s="3">
-        <v>0.5625</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E21" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I21" t="s">
         <v>13</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>44260</v>
+        <v>40972</v>
       </c>
       <c r="C22" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D22" s="3">
-        <v>0.625</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="E22" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>4.166666666666663E-2</v>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K22" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>44261</v>
+        <v>40972</v>
       </c>
       <c r="C23" s="3">
-        <v>0.75</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="D23" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E23" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H23" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I23" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
-        <v>44264</v>
+        <v>40972</v>
       </c>
       <c r="C24" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D24" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E24" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>3.125E-2</v>
+        <v>3.1249999999999944E-2</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="I24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
-        <v>44265</v>
+        <v>44260</v>
       </c>
       <c r="C25" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D25" s="3">
         <v>0.5625</v>
       </c>
-      <c r="D25" s="3">
-        <v>0.625</v>
-      </c>
       <c r="E25" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>6.25E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
@@ -1319,31 +1354,31 @@
         <v>35</v>
       </c>
       <c r="H25" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="I25" t="s">
         <v>13</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>44265</v>
+        <v>44260</v>
       </c>
       <c r="C26" s="3">
-        <v>0.72916666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D26" s="3">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="E26" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
@@ -1352,31 +1387,34 @@
         <v>35</v>
       </c>
       <c r="H26" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I26" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
-        <v>44265</v>
+        <v>44261</v>
       </c>
       <c r="C27" s="3">
         <v>0.75</v>
       </c>
       <c r="D27" s="3">
-        <v>0.78125</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="E27" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>3.125E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F27" t="s">
         <v>29</v>
@@ -1391,25 +1429,25 @@
         <v>31</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
-        <v>44266</v>
+        <v>44264</v>
       </c>
       <c r="C28" s="3">
-        <v>0.375</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D28" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="E28" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v>1.0416666666666685E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="F28" t="s">
         <v>29</v>
@@ -1418,68 +1456,386 @@
         <v>35</v>
       </c>
       <c r="H28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E29" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E30" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" t="s">
         <v>50</v>
       </c>
-      <c r="I28" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="2" t="s">
+      <c r="I30" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="E31" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E32" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E29" s="3" t="str">
+    <row r="33" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="E33" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="E34" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E35" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E36" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="E37" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I37" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="E38" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E39" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I39" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E40" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E30" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E31" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E32" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E37" s="3" t="str">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E41" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Fait qu'on ne peut pas retoucher une case
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4CFE39-6B9E-4980-9D4C-D169BF914F6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF767DF9-8058-4E2E-9419-186665D99C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>J'ai rajouter dans mes regle les casse de couleur</t>
+  </si>
+  <si>
+    <t>J'ai fait en sorte qu'on puisse pas toucher 2 fois une casse</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,10 +1831,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E40" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="40" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Utilisation de lettre au lieu de chiffre pour les coordonées
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF767DF9-8058-4E2E-9419-186665D99C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA6833C-559E-414B-BB6E-650E15716D26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>J'ai fait en sorte qu'on puisse pas toucher 2 fois une casse</t>
+  </si>
+  <si>
+    <t>J'ai fait qu'on introduisse des coordée avec A1 plutôt que 1-1</t>
   </si>
 </sst>
 </file>
@@ -343,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L41" totalsRowShown="0">
-  <autoFilter ref="B4:L41" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L42" totalsRowShown="0">
+  <autoFilter ref="B4:L42" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -627,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L41"/>
+  <dimension ref="B4:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,8 +1867,40 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E41" s="3" t="str">
+    <row r="41" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F41" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" t="s">
+        <v>50</v>
+      </c>
+      <c r="I41" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>44266</v>
+      </c>
+      <c r="E42" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Amélioration de la vérification des données
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7350F052-9FAD-43F0-8F84-4501ABFF959E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801CDC20-81B6-4E39-87A1-ADBB3921AB3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>J'ai fait que les coordonnée soit verifier, qu'on ne puisse pas mettre n'importe quoi.</t>
+  </si>
+  <si>
+    <t>J'ai améliorer la vérification des coordonnées</t>
   </si>
 </sst>
 </file>
@@ -349,8 +352,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L42" totalsRowShown="0">
-  <autoFilter ref="B4:L42" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L43" totalsRowShown="0">
+  <autoFilter ref="B4:L43" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -633,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L42"/>
+  <dimension ref="B4:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1609,7 +1612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>44266</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>44266</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>44266</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>44266</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>44266</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>44266</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>44266</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>44266</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>44266</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>44266</v>
       </c>
@@ -1930,6 +1933,42 @@
       </c>
       <c r="K42" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>44267</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E43" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K43" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise en forme du code / texte
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801CDC20-81B6-4E39-87A1-ADBB3921AB3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7C7F86-7E36-47FD-83CE-488773BE8066}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>J'ai améliorer la vérification des coordonnées</t>
+  </si>
+  <si>
+    <t>Mise au propre</t>
+  </si>
+  <si>
+    <t>J'ai corrigé d es fautes d'orthgraphe, ajouter des legends et aussi bien placer mes bateau</t>
   </si>
 </sst>
 </file>
@@ -352,8 +358,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L43" totalsRowShown="0">
-  <autoFilter ref="B4:L43" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L44" totalsRowShown="0">
+  <autoFilter ref="B4:L44" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L43"/>
+  <dimension ref="B4:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1971,6 +1977,39 @@
         <v>16</v>
       </c>
     </row>
+    <row r="44" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
+        <v>44267</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="E44" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K44" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Mise au propre + Ajout du calcul du score et ajout dans les règle
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE468511-E7DC-4F0B-BAB6-502D8E702351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C94DA73-4A84-4584-9E52-C3AF43279A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,15 @@
   </si>
   <si>
     <t>J'ai réparer mon menu, quand on m'était des lettre dans le chois il crashait</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai changer de place quellque variable </t>
+  </si>
+  <si>
+    <t>J'ai crée une fonction qui calcule les scores et j'ai ajouter dans les regle comment le score est calculer</t>
   </si>
 </sst>
 </file>
@@ -370,8 +379,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L47" totalsRowShown="0">
-  <autoFilter ref="B4:L47" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L49" totalsRowShown="0">
+  <autoFilter ref="B4:L49" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -654,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L47"/>
+  <dimension ref="B4:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2093,10 +2102,10 @@
         <v>44272</v>
       </c>
       <c r="C47" s="3">
-        <v>0.625</v>
+        <v>0.5625</v>
       </c>
       <c r="D47" s="3">
-        <v>0.64583333333333337</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E47" s="3">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
@@ -2119,6 +2128,72 @@
       </c>
       <c r="K47" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <v>44272</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E48" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>44272</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E49" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" t="s">
+        <v>80</v>
+      </c>
+      <c r="I49" t="s">
+        <v>13</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajoute du Scénario teste
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C94DA73-4A84-4584-9E52-C3AF43279A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B5E908-9806-48E9-9A96-4F8CEAE1FE99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,42 @@
   </si>
   <si>
     <t>J'ai crée une fonction qui calcule les scores et j'ai ajouter dans les regle comment le score est calculer</t>
+  </si>
+  <si>
+    <t>13h45</t>
+  </si>
+  <si>
+    <t>Scéanrio teste</t>
+  </si>
+  <si>
+    <t>On a fait un ex, on a parler en anglais de quelle est le meilleur moyen de tester un jeu ?</t>
+  </si>
+  <si>
+    <t>On a regrouper nos réponse et M viret nous a mieu expliquer la théorie</t>
+  </si>
+  <si>
+    <t>On fait un ex sur quelle est le meilleur moyen de tester une calculette</t>
+  </si>
+  <si>
+    <t>On a  mis en commun nos réponse pour tester la calculette et on a éllaborer le meilleur moyen de tester la bataille navale</t>
+  </si>
+  <si>
+    <t>Méthode Smart</t>
+  </si>
+  <si>
+    <t>On a revue des question du questionnaire moodle et ensuite discuter si elle était SMART ou pas</t>
+  </si>
+  <si>
+    <t>J'ai commencer a renommer mes Issues Github</t>
+  </si>
+  <si>
+    <t>J'ai terminer de renommer mes Issues Github</t>
+  </si>
+  <si>
+    <t>Scénario teste</t>
+  </si>
+  <si>
+    <t>J'ai commencer mon scénario teste</t>
   </si>
 </sst>
 </file>
@@ -379,8 +415,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L49" totalsRowShown="0">
-  <autoFilter ref="B4:L49" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L62" totalsRowShown="0">
+  <autoFilter ref="B4:L62" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -663,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L49"/>
+  <dimension ref="B4:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="87" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2193,7 +2229,306 @@
         <v>87</v>
       </c>
       <c r="K49" t="s">
-        <v>58</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E50" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" t="s">
+        <v>90</v>
+      </c>
+      <c r="I50" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E51" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="E52" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>41</v>
+      </c>
+      <c r="H52" t="s">
+        <v>90</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E53" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>90</v>
+      </c>
+      <c r="I53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E54" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E55" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="s">
+        <v>12</v>
+      </c>
+      <c r="I55" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B56" s="1">
+        <v>44274</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E56" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>44274</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E57" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E58" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E59" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E60" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E61" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E62" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reinitialise le tableau des bateau touché
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B5E908-9806-48E9-9A96-4F8CEAE1FE99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7848B991-933D-48B9-BA61-73B39D3CFED8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -305,9 +305,6 @@
     <t>J'ai crée une fonction qui calcule les scores et j'ai ajouter dans les regle comment le score est calculer</t>
   </si>
   <si>
-    <t>13h45</t>
-  </si>
-  <si>
     <t>Scéanrio teste</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>J'ai commencer mon scénario teste</t>
+  </si>
+  <si>
+    <t>J'ai crée une fonction qui reinitialise le tableau des bateaux touché</t>
   </si>
 </sst>
 </file>
@@ -699,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L70"/>
+  <dimension ref="B4:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="87" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="62" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,13 +2253,13 @@
         <v>41</v>
       </c>
       <c r="H50" t="s">
+        <v>89</v>
+      </c>
+      <c r="I50" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="I50" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="K50" t="s">
         <v>15</v>
@@ -2286,13 +2286,13 @@
         <v>11</v>
       </c>
       <c r="H51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I51" t="s">
         <v>13</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K51" t="s">
         <v>15</v>
@@ -2319,13 +2319,13 @@
         <v>41</v>
       </c>
       <c r="H52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I52" t="s">
         <v>13</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K52" t="s">
         <v>15</v>
@@ -2352,13 +2352,13 @@
         <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K53" t="s">
         <v>15</v>
@@ -2385,13 +2385,13 @@
         <v>11</v>
       </c>
       <c r="H54" t="s">
+        <v>94</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="I54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="K54" t="s">
         <v>15</v>
@@ -2424,7 +2424,7 @@
         <v>13</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K55" t="s">
         <v>28</v>
@@ -2457,7 +2457,7 @@
         <v>13</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K56" t="s">
         <v>15</v>
@@ -2484,22 +2484,49 @@
         <v>17</v>
       </c>
       <c r="H57" t="s">
+        <v>98</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="I57" t="s">
-        <v>13</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="K57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E58" s="3" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
-        <v/>
+    <row r="58" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B58" s="1">
+        <v>44279</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E58" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" t="s">
+        <v>35</v>
+      </c>
+      <c r="H58" t="s">
+        <v>50</v>
+      </c>
+      <c r="I58" t="s">
+        <v>13</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K58" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
@@ -2524,11 +2551,6 @@
       <c r="E62" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G70" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commencement du tableau des scores
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Journal_de_travaille.xlsx
+++ b/Doccument_théorique/Journal_de_travaille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797DF35F-F599-47F6-AD2B-E98B6B6838AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344236E-0028-4A15-8D1A-F548FBD5B9FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -348,6 +348,21 @@
   </si>
   <si>
     <t>J'ai chercher comment enregistrer une variable dans un fichier texte a part et j'ai crée une fonction que fait ca</t>
+  </si>
+  <si>
+    <t>Authentification</t>
+  </si>
+  <si>
+    <t>J'ai fait une fonction qui demande le pseudo a l'utilisateur</t>
+  </si>
+  <si>
+    <t>J'ai completer la fonction pour s'authentifier, elle demande a l'tuilisateur si il est sur de son pseudo</t>
+  </si>
+  <si>
+    <t>Tableau des scores</t>
+  </si>
+  <si>
+    <t>J'ai commencer le tableau des score, j'ai fait une en tete</t>
   </si>
 </sst>
 </file>
@@ -424,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L62" totalsRowShown="0">
-  <autoFilter ref="B4:L62" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B485EC57-35FF-4539-9109-8C783E6E7498}" name="Tableau1" displayName="Tableau1" ref="B4:L66" totalsRowShown="0">
+  <autoFilter ref="B4:L66" xr:uid="{144B54FC-3B12-44C0-ADF1-69A36A3D9E09}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C69ED52E-80E1-46D1-826B-7C09729DC6AB}" name="Date"/>
     <tableColumn id="2" xr3:uid="{6EC05AA0-8731-47A4-928E-3C03985874D4}" name="Heure début" dataDxfId="3"/>
@@ -708,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:L62"/>
+  <dimension ref="B4:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="62" workbookViewId="0">
-      <selection activeCell="X47" sqref="X47"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="62" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2604,14 +2619,119 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E61" s="3" t="str">
+    <row r="61" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>44286</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E61" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" t="s">
+        <v>35</v>
+      </c>
+      <c r="H61" t="s">
+        <v>104</v>
+      </c>
+      <c r="I61" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>44286</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E62" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" t="s">
+        <v>35</v>
+      </c>
+      <c r="H62" t="s">
+        <v>104</v>
+      </c>
+      <c r="I62" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
+        <v>44286</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E63" s="3">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" t="s">
+        <v>35</v>
+      </c>
+      <c r="H63" t="s">
+        <v>107</v>
+      </c>
+      <c r="I63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E64" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E62" s="3" t="str">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="3" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="3" t="str">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure fin]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure début]])</f>
         <v/>
       </c>

</xml_diff>